<commit_message>
Refactor method names and update parameter types for clarity; enhance debug logging functionality
</commit_message>
<xml_diff>
--- a/test_e2e/main-treasury-temp/user_data__no_settings/data.xlsx
+++ b/test_e2e/main-treasury-temp/user_data__no_settings/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\tests\_end_to_end_tests\main-treasury-temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\test_e2e\main-treasury-temp\user_data__no_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E8E9AE-8C96-49E5-A348-CA35958A98D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9DB201-81DD-4C27-AF61-F94A11E1C7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Nominativo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>descrizione</t>
   </si>
@@ -81,6 +78,15 @@
   </si>
   <si>
     <t>amount delta value</t>
+  </si>
+  <si>
+    <t>simulation input</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>inactive</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -185,6 +191,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -193,7 +200,28 @@
     <cellStyle name="Comma 2 3" xfId="1" xr:uid="{D614F647-4E31-4F6F-A208-E19F25DAA59C}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -244,15 +272,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A12:C14" totalsRowShown="0" headerRowBorderDxfId="3">
-  <autoFilter ref="A12:C14" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:B14">
-    <sortCondition descending="1" ref="B12:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A12:G14" totalsRowShown="0" headerRowBorderDxfId="5">
+  <autoFilter ref="A12:G14" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B13:E14">
+    <sortCondition descending="1" ref="E12:E14"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="Nominativo"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="0"/>
+  <tableColumns count="7">
+    <tableColumn id="3" xr3:uid="{B21D81C7-F42B-44FC-B1F0-C32FFAECE00E}" name="inactive"/>
+    <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="simulation input"/>
+    <tableColumn id="8" xr3:uid="{01EC1143-3540-4624-827E-FAD2B2210C97}" name="type"/>
+    <tableColumn id="7" xr3:uid="{71D759DF-9CEC-44FE-9285-ABB1DFF9D850}" name="vs type"/>
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{28A3B7BE-40FF-4AAE-A2F7-CFB35D699FD5}" name="nome" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -270,9 +302,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +342,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -416,7 +448,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -558,7 +590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,49 +598,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D13926F-0BD1-460D-BBDD-36F9AE527C93}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="15.54296875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="68.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.1796875" customWidth="1"/>
-    <col min="7" max="7" width="49.08984375" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -616,82 +648,97 @@
       <c r="C5"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13" s="3">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3">
-        <v>100</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14" s="3">
         <v>150</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F14" s="3"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>

</xml_diff>

<commit_message>
Add DEFAULT_ACCOUNTING_VS_TYPE to globals; rename leger_utils to square_trn and refactor related functions
</commit_message>
<xml_diff>
--- a/test_e2e/main-treasury-temp/user_data__no_settings/data.xlsx
+++ b/test_e2e/main-treasury-temp/user_data__no_settings/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\test_e2e\main-treasury-temp\user_data__no_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9DB201-81DD-4C27-AF61-F94A11E1C7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8F5102-FF5A-410C-AD39-34106EDD5AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -80,13 +80,13 @@
     <t>amount delta value</t>
   </si>
   <si>
-    <t>simulation input</t>
-  </si>
-  <si>
-    <t>nome</t>
-  </si>
-  <si>
     <t>inactive</t>
+  </si>
+  <si>
+    <t>simulation input2</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -200,7 +200,25 @@
     <cellStyle name="Comma 2 3" xfId="1" xr:uid="{D614F647-4E31-4F6F-A208-E19F25DAA59C}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -272,19 +290,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A12:G14" totalsRowShown="0" headerRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}" name="CO__crediti2022" displayName="CO__crediti2022" ref="A12:G14" totalsRowShown="0" headerRowBorderDxfId="6">
   <autoFilter ref="A12:G14" xr:uid="{34163CA1-1061-49B7-9340-36818410973A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B13:E14">
     <sortCondition descending="1" ref="E12:E14"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="3" xr3:uid="{B21D81C7-F42B-44FC-B1F0-C32FFAECE00E}" name="inactive"/>
-    <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="simulation input"/>
+    <tableColumn id="1" xr3:uid="{9B0BE50A-5079-4DCD-90F2-19056CCF5E2E}" name="name" dataDxfId="0" dataCellStyle="Comma"/>
     <tableColumn id="8" xr3:uid="{01EC1143-3540-4624-827E-FAD2B2210C97}" name="type"/>
     <tableColumn id="7" xr3:uid="{71D759DF-9CEC-44FE-9285-ABB1DFF9D850}" name="vs type"/>
-    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{28A3B7BE-40FF-4AAE-A2F7-CFB35D699FD5}" name="nome" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4FE7BDEF-BAD8-40B6-8054-1B7BF024310B}" name="#2022-12-31" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="10" xr3:uid="{FABACAE9-0133-4DAF-9F3F-2F22A207B458}" name="simulation input2" dataDxfId="1" totalsRowDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{86687EC0-6300-489A-A6CB-48340095E159}" name="descrizione" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -601,7 +619,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,7 +627,7 @@
     <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="15.54296875" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -693,10 +711,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1</v>
@@ -707,7 +725,7 @@
       <c r="E12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -715,27 +733,25 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13" s="3">
         <v>100</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14" s="3">
         <v>150</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
       <c r="G14" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>